<commit_message>
resolved the bug in for loop
</commit_message>
<xml_diff>
--- a/Data Cleaning/nutritionixAPI/withNutrients.xlsx
+++ b/Data Cleaning/nutritionixAPI/withNutrients.xlsx
@@ -9946,6 +9946,21 @@
       <c r="I202" t="n">
         <v>152.55</v>
       </c>
+      <c r="J202" t="n">
+        <v>74.45</v>
+      </c>
+      <c r="K202" t="n">
+        <v>477.14</v>
+      </c>
+      <c r="L202" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="M202" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="N202" t="n">
+        <v>21.21</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
@@ -9976,6 +9991,21 @@
       <c r="I203" t="n">
         <v>219.6</v>
       </c>
+      <c r="J203" t="n">
+        <v>51.45</v>
+      </c>
+      <c r="K203" t="n">
+        <v>501.2400000000001</v>
+      </c>
+      <c r="L203" t="n">
+        <v>20.83</v>
+      </c>
+      <c r="M203" t="n">
+        <v>18.13</v>
+      </c>
+      <c r="N203" t="n">
+        <v>39.99999999999999</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
@@ -10006,6 +10036,21 @@
       <c r="I204" t="n">
         <v>279.9</v>
       </c>
+      <c r="J204" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="K204" t="n">
+        <v>573.9300000000001</v>
+      </c>
+      <c r="L204" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="M204" t="n">
+        <v>29.29</v>
+      </c>
+      <c r="N204" t="n">
+        <v>65.01000000000001</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
@@ -10034,6 +10079,21 @@
       </c>
       <c r="I205" t="n">
         <v>240.3</v>
+      </c>
+      <c r="J205" t="n">
+        <v>74.45</v>
+      </c>
+      <c r="K205" t="n">
+        <v>477.14</v>
+      </c>
+      <c r="L205" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="M205" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="N205" t="n">
+        <v>21.21</v>
       </c>
     </row>
     <row r="206">
@@ -10065,6 +10125,21 @@
       <c r="I206" t="n">
         <v>205.65</v>
       </c>
+      <c r="J206" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="K206" t="n">
+        <v>759.0000000000001</v>
+      </c>
+      <c r="L206" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="M206" t="n">
+        <v>52.18</v>
+      </c>
+      <c r="N206" t="n">
+        <v>53.45</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
@@ -10095,6 +10170,21 @@
       <c r="I207" t="n">
         <v>245.7</v>
       </c>
+      <c r="J207" t="n">
+        <v>18.57</v>
+      </c>
+      <c r="K207" t="n">
+        <v>606.45</v>
+      </c>
+      <c r="L207" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="M207" t="n">
+        <v>22.14</v>
+      </c>
+      <c r="N207" t="n">
+        <v>84.39999999999999</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
@@ -10123,6 +10213,21 @@
       </c>
       <c r="I208" t="n">
         <v>134.55</v>
+      </c>
+      <c r="J208" t="n">
+        <v>74.45</v>
+      </c>
+      <c r="K208" t="n">
+        <v>477.14</v>
+      </c>
+      <c r="L208" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="M208" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="N208" t="n">
+        <v>21.21</v>
       </c>
     </row>
     <row r="209">
@@ -10154,6 +10259,21 @@
       <c r="I209" t="n">
         <v>262.8</v>
       </c>
+      <c r="J209" t="n">
+        <v>78.17999999999999</v>
+      </c>
+      <c r="K209" t="n">
+        <v>567.3299999999999</v>
+      </c>
+      <c r="L209" t="n">
+        <v>23.08</v>
+      </c>
+      <c r="M209" t="n">
+        <v>15.69</v>
+      </c>
+      <c r="N209" t="n">
+        <v>34.35</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
@@ -10184,6 +10304,21 @@
       <c r="I210" t="n">
         <v>225.9</v>
       </c>
+      <c r="J210" t="n">
+        <v>23.74</v>
+      </c>
+      <c r="K210" t="n">
+        <v>436.6200000000001</v>
+      </c>
+      <c r="L210" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="M210" t="n">
+        <v>25.51</v>
+      </c>
+      <c r="N210" t="n">
+        <v>29.87</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
@@ -10212,6 +10347,21 @@
       </c>
       <c r="I211" t="n">
         <v>205.2</v>
+      </c>
+      <c r="J211" t="n">
+        <v>80</v>
+      </c>
+      <c r="K211" t="n">
+        <v>508.54</v>
+      </c>
+      <c r="L211" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="M211" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="N211" t="n">
+        <v>22.32</v>
       </c>
     </row>
     <row r="212">
@@ -10243,6 +10393,21 @@
       <c r="I212" t="n">
         <v>177.75</v>
       </c>
+      <c r="J212" t="n">
+        <v>12.59</v>
+      </c>
+      <c r="K212" t="n">
+        <v>306.63</v>
+      </c>
+      <c r="L212" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="M212" t="n">
+        <v>18.82</v>
+      </c>
+      <c r="N212" t="n">
+        <v>23.2</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
@@ -10273,6 +10438,21 @@
       <c r="I213" t="n">
         <v>111.6</v>
       </c>
+      <c r="J213" t="n">
+        <v>30.18</v>
+      </c>
+      <c r="K213" t="n">
+        <v>650.9100000000001</v>
+      </c>
+      <c r="L213" t="n">
+        <v>15.85</v>
+      </c>
+      <c r="M213" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="N213" t="n">
+        <v>91.70999999999999</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
@@ -10301,6 +10481,21 @@
       </c>
       <c r="I214" t="n">
         <v>172.8</v>
+      </c>
+      <c r="J214" t="n">
+        <v>77.47999999999999</v>
+      </c>
+      <c r="K214" t="n">
+        <v>503.11</v>
+      </c>
+      <c r="L214" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="M214" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="N214" t="n">
+        <v>22.62</v>
       </c>
     </row>
     <row r="215">
@@ -10332,6 +10527,21 @@
       <c r="I215" t="n">
         <v>211.05</v>
       </c>
+      <c r="J215" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="K215" t="n">
+        <v>437.6</v>
+      </c>
+      <c r="L215" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="M215" t="n">
+        <v>21.82</v>
+      </c>
+      <c r="N215" t="n">
+        <v>55.73</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
@@ -10362,6 +10572,21 @@
       <c r="I216" t="n">
         <v>172.35</v>
       </c>
+      <c r="J216" t="n">
+        <v>16</v>
+      </c>
+      <c r="K216" t="n">
+        <v>474.71</v>
+      </c>
+      <c r="L216" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="M216" t="n">
+        <v>24.07</v>
+      </c>
+      <c r="N216" t="n">
+        <v>49.23</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
@@ -10390,6 +10615,21 @@
       </c>
       <c r="I217" t="n">
         <v>197.55</v>
+      </c>
+      <c r="J217" t="n">
+        <v>75.56999999999999</v>
+      </c>
+      <c r="K217" t="n">
+        <v>486.03</v>
+      </c>
+      <c r="L217" t="n">
+        <v>7.87</v>
+      </c>
+      <c r="M217" t="n">
+        <v>10.11</v>
+      </c>
+      <c r="N217" t="n">
+        <v>21.64</v>
       </c>
     </row>
     <row r="218">
@@ -10421,6 +10661,21 @@
       <c r="I218" t="n">
         <v>190.8</v>
       </c>
+      <c r="J218" t="n">
+        <v>51.39</v>
+      </c>
+      <c r="K218" t="n">
+        <v>616.6099999999999</v>
+      </c>
+      <c r="L218" t="n">
+        <v>16.48</v>
+      </c>
+      <c r="M218" t="n">
+        <v>19.01</v>
+      </c>
+      <c r="N218" t="n">
+        <v>58.56</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
@@ -10451,6 +10706,21 @@
       <c r="I219" t="n">
         <v>200.7</v>
       </c>
+      <c r="J219" t="n">
+        <v>57.28</v>
+      </c>
+      <c r="K219" t="n">
+        <v>712.3099999999999</v>
+      </c>
+      <c r="L219" t="n">
+        <v>12.92</v>
+      </c>
+      <c r="M219" t="n">
+        <v>30.72</v>
+      </c>
+      <c r="N219" t="n">
+        <v>51.00000000000001</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
@@ -10479,6 +10749,21 @@
       </c>
       <c r="I220" t="n">
         <v>182.7</v>
+      </c>
+      <c r="J220" t="n">
+        <v>42.14</v>
+      </c>
+      <c r="K220" t="n">
+        <v>300.65</v>
+      </c>
+      <c r="L220" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="M220" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="N220" t="n">
+        <v>14.5</v>
       </c>
     </row>
     <row r="221">
@@ -10511,6 +10796,21 @@
       <c r="I221" t="n">
         <v>154.35</v>
       </c>
+      <c r="J221" t="n">
+        <v>13.77</v>
+      </c>
+      <c r="K221" t="n">
+        <v>163.4</v>
+      </c>
+      <c r="L221" t="n">
+        <v>4.720000000000001</v>
+      </c>
+      <c r="M221" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="N221" t="n">
+        <v>13.54</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
@@ -10542,6 +10842,21 @@
       <c r="I222" t="n">
         <v>162.45</v>
       </c>
+      <c r="J222" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="K222" t="n">
+        <v>442.77</v>
+      </c>
+      <c r="L222" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="M222" t="n">
+        <v>22.04</v>
+      </c>
+      <c r="N222" t="n">
+        <v>51.19</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
@@ -10573,6 +10888,21 @@
       <c r="I223" t="n">
         <v>243</v>
       </c>
+      <c r="J223" t="n">
+        <v>33.47</v>
+      </c>
+      <c r="K223" t="n">
+        <v>287.63</v>
+      </c>
+      <c r="L223" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="M223" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="N223" t="n">
+        <v>16.03</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
@@ -10602,6 +10932,21 @@
       </c>
       <c r="I224" t="n">
         <v>162</v>
+      </c>
+      <c r="J224" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="K224" t="n">
+        <v>113.9</v>
+      </c>
+      <c r="L224" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M224" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="N224" t="n">
+        <v>21.56</v>
       </c>
     </row>
     <row r="225">
@@ -10633,6 +10978,21 @@
       </c>
       <c r="I225" t="n">
         <v>184.5</v>
+      </c>
+      <c r="J225" t="n">
+        <v>6.890000000000001</v>
+      </c>
+      <c r="K225" t="n">
+        <v>187.65</v>
+      </c>
+      <c r="L225" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="M225" t="n">
+        <v>10.61</v>
+      </c>
+      <c r="N225" t="n">
+        <v>17.29</v>
       </c>
     </row>
     <row r="226">
@@ -10666,6 +11026,21 @@
       <c r="I226" t="n">
         <v>249.3</v>
       </c>
+      <c r="J226" t="n">
+        <v>42.11</v>
+      </c>
+      <c r="K226" t="n">
+        <v>398.75</v>
+      </c>
+      <c r="L226" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="M226" t="n">
+        <v>20.03</v>
+      </c>
+      <c r="N226" t="n">
+        <v>15.65</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
@@ -10697,6 +11072,21 @@
       <c r="I227" t="n">
         <v>131.4</v>
       </c>
+      <c r="J227" t="n">
+        <v>7.34</v>
+      </c>
+      <c r="K227" t="n">
+        <v>202</v>
+      </c>
+      <c r="L227" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M227" t="n">
+        <v>7.47</v>
+      </c>
+      <c r="N227" t="n">
+        <v>24.8</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
@@ -10726,6 +11116,21 @@
       </c>
       <c r="I228" t="n">
         <v>137.7</v>
+      </c>
+      <c r="J228" t="n">
+        <v>34.68</v>
+      </c>
+      <c r="K228" t="n">
+        <v>338</v>
+      </c>
+      <c r="L228" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="M228" t="n">
+        <v>15.58</v>
+      </c>
+      <c r="N228" t="n">
+        <v>14.91</v>
       </c>
     </row>
     <row r="229">
@@ -10758,6 +11163,21 @@
       <c r="I229" t="n">
         <v>270</v>
       </c>
+      <c r="J229" t="n">
+        <v>21.16</v>
+      </c>
+      <c r="K229" t="n">
+        <v>244.96</v>
+      </c>
+      <c r="L229" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="M229" t="n">
+        <v>14.41</v>
+      </c>
+      <c r="N229" t="n">
+        <v>9.31</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
@@ -10787,6 +11207,21 @@
       </c>
       <c r="I230" t="n">
         <v>167.85</v>
+      </c>
+      <c r="J230" t="n">
+        <v>60.13999999999999</v>
+      </c>
+      <c r="K230" t="n">
+        <v>377.23</v>
+      </c>
+      <c r="L230" t="n">
+        <v>9</v>
+      </c>
+      <c r="M230" t="n">
+        <v>9.039999999999999</v>
+      </c>
+      <c r="N230" t="n">
+        <v>16.85</v>
       </c>
     </row>
     <row r="231">
@@ -10819,6 +11254,21 @@
       <c r="I231" t="n">
         <v>200.25</v>
       </c>
+      <c r="J231" t="n">
+        <v>19.02</v>
+      </c>
+      <c r="K231" t="n">
+        <v>288.2</v>
+      </c>
+      <c r="L231" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M231" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="N231" t="n">
+        <v>15.71</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
@@ -10850,6 +11300,21 @@
       <c r="I232" t="n">
         <v>243</v>
       </c>
+      <c r="J232" t="n">
+        <v>62.22</v>
+      </c>
+      <c r="K232" t="n">
+        <v>440.61</v>
+      </c>
+      <c r="L232" t="n">
+        <v>6.37</v>
+      </c>
+      <c r="M232" t="n">
+        <v>12.02</v>
+      </c>
+      <c r="N232" t="n">
+        <v>23.66</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
@@ -10881,6 +11346,21 @@
       <c r="I233" t="n">
         <v>142.2</v>
       </c>
+      <c r="J233" t="n">
+        <v>40.75</v>
+      </c>
+      <c r="K233" t="n">
+        <v>245.5</v>
+      </c>
+      <c r="L233" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="M233" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="N233" t="n">
+        <v>16.38</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
@@ -10911,6 +11391,21 @@
       </c>
       <c r="I234" t="n">
         <v>188.1</v>
+      </c>
+      <c r="J234" t="n">
+        <v>40.75</v>
+      </c>
+      <c r="K234" t="n">
+        <v>350</v>
+      </c>
+      <c r="L234" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="M234" t="n">
+        <v>14.49</v>
+      </c>
+      <c r="N234" t="n">
+        <v>12.79</v>
       </c>
     </row>
     <row r="235">
@@ -10944,6 +11439,21 @@
       <c r="I235" t="n">
         <v>274.95</v>
       </c>
+      <c r="J235" t="n">
+        <v>60.26</v>
+      </c>
+      <c r="K235" t="n">
+        <v>432.75</v>
+      </c>
+      <c r="L235" t="n">
+        <v>7.01</v>
+      </c>
+      <c r="M235" t="n">
+        <v>12.32</v>
+      </c>
+      <c r="N235" t="n">
+        <v>22.78</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
@@ -10974,6 +11484,21 @@
       </c>
       <c r="I236" t="n">
         <v>121.95</v>
+      </c>
+      <c r="J236" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="K236" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="L236" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="M236" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="N236" t="n">
+        <v>17.21</v>
       </c>
     </row>
     <row r="237">
@@ -11008,6 +11533,21 @@
       <c r="I237" t="n">
         <v>165.15</v>
       </c>
+      <c r="J237" t="n">
+        <v>71.23999999999999</v>
+      </c>
+      <c r="K237" t="n">
+        <v>642.6999999999999</v>
+      </c>
+      <c r="L237" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="M237" t="n">
+        <v>27.07999999999999</v>
+      </c>
+      <c r="N237" t="n">
+        <v>30.74</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
@@ -11040,6 +11580,21 @@
       <c r="I238" t="n">
         <v>245.25</v>
       </c>
+      <c r="J238" t="n">
+        <v>60.26</v>
+      </c>
+      <c r="K238" t="n">
+        <v>432.75</v>
+      </c>
+      <c r="L238" t="n">
+        <v>7.01</v>
+      </c>
+      <c r="M238" t="n">
+        <v>12.32</v>
+      </c>
+      <c r="N238" t="n">
+        <v>22.78</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
@@ -11069,6 +11624,21 @@
       </c>
       <c r="I239" t="n">
         <v>160.2</v>
+      </c>
+      <c r="J239" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="K239" t="n">
+        <v>209</v>
+      </c>
+      <c r="L239" t="n">
+        <v>3</v>
+      </c>
+      <c r="M239" t="n">
+        <v>14.31</v>
+      </c>
+      <c r="N239" t="n">
+        <v>11.26</v>
       </c>
     </row>
     <row r="240">
@@ -11101,6 +11671,21 @@
       <c r="I240" t="n">
         <v>175.5</v>
       </c>
+      <c r="J240" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="K240" t="n">
+        <v>625.54</v>
+      </c>
+      <c r="L240" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="M240" t="n">
+        <v>50.29</v>
+      </c>
+      <c r="N240" t="n">
+        <v>35.93</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
@@ -11132,6 +11717,21 @@
       <c r="I241" t="n">
         <v>212.4</v>
       </c>
+      <c r="J241" t="n">
+        <v>56.56</v>
+      </c>
+      <c r="K241" t="n">
+        <v>343.2</v>
+      </c>
+      <c r="L241" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="M241" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="N241" t="n">
+        <v>16.29</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
@@ -11160,6 +11760,21 @@
       </c>
       <c r="I242" t="n">
         <v>143.55</v>
+      </c>
+      <c r="J242" t="n">
+        <v>22.63</v>
+      </c>
+      <c r="K242" t="n">
+        <v>334.1</v>
+      </c>
+      <c r="L242" t="n">
+        <v>4</v>
+      </c>
+      <c r="M242" t="n">
+        <v>9.140000000000001</v>
+      </c>
+      <c r="N242" t="n">
+        <v>38.89</v>
       </c>
     </row>
     <row r="243">
@@ -11192,6 +11807,21 @@
       <c r="I243" t="n">
         <v>84.60000000000001</v>
       </c>
+      <c r="J243" t="n">
+        <v>11.26</v>
+      </c>
+      <c r="K243" t="n">
+        <v>58</v>
+      </c>
+      <c r="L243" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="M243" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N243" t="n">
+        <v>3.44</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
@@ -11219,6 +11849,21 @@
       </c>
       <c r="I244" t="n">
         <v>87.75</v>
+      </c>
+      <c r="J244" t="n">
+        <v>0</v>
+      </c>
+      <c r="K244" t="n">
+        <v>64</v>
+      </c>
+      <c r="L244" t="n">
+        <v>0</v>
+      </c>
+      <c r="M244" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="N244" t="n">
+        <v>13.08</v>
       </c>
     </row>
     <row r="245">
@@ -11252,6 +11897,21 @@
       <c r="I245" t="n">
         <v>169.2</v>
       </c>
+      <c r="J245" t="n">
+        <v>33.73</v>
+      </c>
+      <c r="K245" t="n">
+        <v>293.85</v>
+      </c>
+      <c r="L245" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="M245" t="n">
+        <v>9.66</v>
+      </c>
+      <c r="N245" t="n">
+        <v>18.58</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
@@ -11281,6 +11941,21 @@
       </c>
       <c r="I246" t="n">
         <v>125.1</v>
+      </c>
+      <c r="J246" t="n">
+        <v>32.63</v>
+      </c>
+      <c r="K246" t="n">
+        <v>343.65</v>
+      </c>
+      <c r="L246" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="M246" t="n">
+        <v>10.03</v>
+      </c>
+      <c r="N246" t="n">
+        <v>28.92</v>
       </c>
     </row>
     <row r="247">
@@ -11314,6 +11989,21 @@
       <c r="I247" t="n">
         <v>125.1</v>
       </c>
+      <c r="J247" t="n">
+        <v>10.92</v>
+      </c>
+      <c r="K247" t="n">
+        <v>233</v>
+      </c>
+      <c r="L247" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="M247" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="N247" t="n">
+        <v>28.11</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="2" t="n">
@@ -11346,6 +12036,21 @@
       <c r="I248" t="n">
         <v>153</v>
       </c>
+      <c r="J248" t="n">
+        <v>30.97</v>
+      </c>
+      <c r="K248" t="n">
+        <v>401.35</v>
+      </c>
+      <c r="L248" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="M248" t="n">
+        <v>16.58</v>
+      </c>
+      <c r="N248" t="n">
+        <v>31.12</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="n">
@@ -11379,6 +12084,21 @@
       </c>
       <c r="I249" t="n">
         <v>181.8</v>
+      </c>
+      <c r="J249" t="n">
+        <v>80.02</v>
+      </c>
+      <c r="K249" t="n">
+        <v>511.4</v>
+      </c>
+      <c r="L249" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="M249" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="N249" t="n">
+        <v>22.57</v>
       </c>
     </row>
     <row r="250">
@@ -11415,6 +12135,21 @@
       <c r="I250" t="n">
         <v>189.45</v>
       </c>
+      <c r="J250" t="n">
+        <v>73.87</v>
+      </c>
+      <c r="K250" t="n">
+        <v>851.85</v>
+      </c>
+      <c r="L250" t="n">
+        <v>24.97</v>
+      </c>
+      <c r="M250" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="N250" t="n">
+        <v>56.61</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="2" t="n">
@@ -11449,6 +12184,21 @@
       </c>
       <c r="I251" t="n">
         <v>172.35</v>
+      </c>
+      <c r="J251" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="K251" t="n">
+        <v>736.4300000000001</v>
+      </c>
+      <c r="L251" t="n">
+        <v>5.199999999999999</v>
+      </c>
+      <c r="M251" t="n">
+        <v>51.70999999999999</v>
+      </c>
+      <c r="N251" t="n">
+        <v>51.90000000000001</v>
       </c>
     </row>
     <row r="252">

</xml_diff>

<commit_message>
added ss for github
</commit_message>
<xml_diff>
--- a/Data Cleaning/nutritionixAPI/withNutrients.xlsx
+++ b/Data Cleaning/nutritionixAPI/withNutrients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thushara Piyasekara\Downloads\IIT\Year 2 Semester 2\SDGP Implementaion\Diabuddies_SDGP\Data Cleaning\nutritionixAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA752751-014F-49D1-BAAC-DB714A2A9445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ED660E-B367-452E-AD04-B3C2DCFC758E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="324" windowWidth="22956" windowHeight="12636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="276" windowWidth="22956" windowHeight="12636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12890,12 +12890,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13200,17 +13203,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="B2495" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B2503" sqref="B2503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="123.6640625" customWidth="1"/>
+    <col min="2" max="2" width="134" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13840,11 +13843,11 @@
         <v>18.16</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44193.518750000003</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
@@ -14460,11 +14463,11 @@
         <v>36.979999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44198.383333333331</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D33" t="s">
@@ -14890,11 +14893,11 @@
         <v>20.309999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44201.508333333331</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E44" t="s">
@@ -14928,11 +14931,11 @@
         <v>11.76</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44201.789583333331</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E45" t="s">
@@ -15007,11 +15010,11 @@
         <v>19.22</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44202.487500000003</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E47" t="s">
@@ -89105,11 +89108,11 @@
         <v>193.95</v>
       </c>
     </row>
-    <row r="2503" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2503" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2503" s="2">
         <v>44153.748611111107</v>
       </c>
-      <c r="B2503" t="s">
+      <c r="B2503" s="3" t="s">
         <v>2456</v>
       </c>
       <c r="E2503" t="s">
@@ -89151,11 +89154,11 @@
         <v>218.25</v>
       </c>
     </row>
-    <row r="2505" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2505" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2505" s="2">
         <v>44154.509027777778</v>
       </c>
-      <c r="B2505" t="s">
+      <c r="B2505" s="3" t="s">
         <v>2458</v>
       </c>
       <c r="E2505" t="s">
@@ -90715,11 +90718,11 @@
         <v>167.4</v>
       </c>
     </row>
-    <row r="2573" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2573" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2573" s="2">
         <v>44164.376388888893</v>
       </c>
-      <c r="B2573" t="s">
+      <c r="B2573" s="3" t="s">
         <v>2525</v>
       </c>
       <c r="E2573" t="s">
@@ -90761,11 +90764,11 @@
         <v>85.949999999999989</v>
       </c>
     </row>
-    <row r="2575" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2575" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A2575" s="2">
         <v>44164.772222222222</v>
       </c>
-      <c r="B2575" t="s">
+      <c r="B2575" s="3" t="s">
         <v>2527</v>
       </c>
       <c r="E2575" t="s">
@@ -90784,11 +90787,11 @@
         <v>94.949999999999989</v>
       </c>
     </row>
-    <row r="2576" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2576" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2576" s="2">
         <v>44165.240972222222</v>
       </c>
-      <c r="B2576" t="s">
+      <c r="B2576" s="3" t="s">
         <v>2528</v>
       </c>
       <c r="E2576" t="s">

</xml_diff>